<commit_message>
delete a unnecessary files
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0E74F0-1C02-4B0C-A0F2-69BD4BD33C9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A7D561-B75C-414A-9F45-65F133CBAA23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>1.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -31,14 +31,6 @@
   </si>
   <si>
     <t>3.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -364,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -459,64 +451,6 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <v>200</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>200</v>
-      </c>
-      <c r="G4">
-        <v>200</v>
-      </c>
-      <c r="H4">
-        <v>100</v>
-      </c>
-      <c r="I4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-      <c r="D5">
-        <v>200</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>200</v>
-      </c>
-      <c r="G5">
-        <v>200</v>
-      </c>
-      <c r="H5">
-        <v>100</v>
-      </c>
-      <c r="I5">
-        <v>200</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>